<commit_message>
Created inventor dir and stls
</commit_message>
<xml_diff>
--- a/inventor/blinds-refs.xlsx
+++ b/inventor/blinds-refs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>wall1_thick</t>
   </si>
@@ -133,6 +133,30 @@
   </si>
   <si>
     <t>armslotd</t>
+  </si>
+  <si>
+    <t>fanhb</t>
+  </si>
+  <si>
+    <t>fanhs</t>
+  </si>
+  <si>
+    <t>adapterwallthick</t>
+  </si>
+  <si>
+    <t>adapterwallslotd</t>
+  </si>
+  <si>
+    <t>armhornthick</t>
+  </si>
+  <si>
+    <t>hornthick</t>
+  </si>
+  <si>
+    <t>hornscrewholed</t>
+  </si>
+  <si>
+    <t>hornscrewheadd</t>
   </si>
 </sst>
 </file>
@@ -464,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -671,7 +695,7 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -706,8 +730,8 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <f>B4 - 18</f>
-        <v>26</v>
+        <f>B4 - 20</f>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -784,6 +808,70 @@
       </c>
       <c r="B36">
         <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inventor stls - make arm fit within walls
</commit_message>
<xml_diff>
--- a/inventor/blinds-refs.xlsx
+++ b/inventor/blinds-refs.xlsx
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -730,8 +730,8 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <f>B4 - 20</f>
-        <v>24</v>
+        <f>B3 - 20</f>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -790,8 +790,8 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <f>B32+2+2</f>
-        <v>36</v>
+        <f>B32+2</f>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2">

</xml_diff>